<commit_message>
11.21 end of day
</commit_message>
<xml_diff>
--- a/Táblázatok/Analog_ORDER.xlsx
+++ b/Táblázatok/Analog_ORDER.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="191">
   <si>
     <t>Ref.Des.</t>
   </si>
@@ -579,9 +579,6 @@
     <t>(1%)</t>
   </si>
   <si>
-    <t>66-OAR1R100FLF</t>
-  </si>
-  <si>
     <t>765731-01</t>
   </si>
   <si>
@@ -589,6 +586,12 @@
   </si>
   <si>
     <t>IRLB3034</t>
+  </si>
+  <si>
+    <t>713244-01</t>
+  </si>
+  <si>
+    <t>silpad</t>
   </si>
 </sst>
 </file>
@@ -660,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
@@ -673,9 +676,10 @@
     <xf numFmtId="17" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -691,7 +695,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -987,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:M70"/>
+  <dimension ref="A5:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,13 +1398,7 @@
         <v>8</v>
       </c>
       <c r="H28" t="s">
-        <v>24</v>
-      </c>
-      <c r="I28" t="s">
-        <v>24</v>
-      </c>
-      <c r="J28" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
@@ -1958,7 +1956,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>111</v>
       </c>
@@ -1966,7 +1964,7 @@
         <v>112</v>
       </c>
       <c r="D65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F65">
         <v>8</v>
@@ -1978,7 +1976,7 @@
         <v>1698299</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>114</v>
       </c>
@@ -1995,7 +1993,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>97</v>
       </c>
@@ -2003,16 +2001,33 @@
         <v>33</v>
       </c>
       <c r="H68" t="s">
+        <v>186</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H69" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H69" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="J69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="H70" s="6"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>190</v>
+      </c>
+      <c r="I72" s="10">
+        <v>681090</v>
+      </c>
+      <c r="J72">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>